<commit_message>
Uploaded the kf data
</commit_message>
<xml_diff>
--- a/project_3/weak_sensor_calib_data.xlsx
+++ b/project_3/weak_sensor_calib_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Merc.MERCURY\Documents\ComputingandControl\project_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D6F516C6-55B3-4A81-B0BA-9EF2EE53CDB6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{168961A7-EEB3-448A-99C4-089833F8C21B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{F69567C1-1741-4674-BADD-EE8C7ED6F8E1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{F69567C1-1741-4674-BADD-EE8C7ED6F8E1}"/>
   </bookViews>
   <sheets>
     <sheet name="6 Inches" sheetId="1" r:id="rId1"/>
@@ -387,8 +387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9EE7C9-5EB0-427C-9E05-CE95D4BCD757}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2866,13 +2866,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB75B0F4-4D7B-4EAC-8A30-C297E67328D0}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>